<commit_message>
Small fix in PS value of "L1_IsoEG32er2p5_Mt40"
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v1_0_0/PrescaleTable/L1Menu_Collisions2022_v1_0_0.xlsx
+++ b/development/L1Menu_Collisions2022_v1_0_0/PrescaleTable/L1Menu_Collisions2022_v1_0_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2022_v1_0_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3462089-46D9-4E47-82B4-98E0BFF09CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0900D7C-71FB-2546-8F9E-AAB9CE8FA3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2541,8 +2541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF3B8E07-BE26-384A-A4B5-1B0A96E53592}">
   <dimension ref="A1:IV382"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A354" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B369" sqref="B369"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A152" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C168" sqref="C168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8408,28 +8408,28 @@
         <v>0</v>
       </c>
       <c r="D168" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E168" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F168" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G168" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H168" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I168" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J168" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K168" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated of PS table for menu v1_0_0
Modifications done:
- activated SingleMu22_EMTF/OMTF/BMTF seeds in the all PS tables (with PS=1)
- activated also the SingleIsoTau35 seed in the PS table for rate studies (in column 0.8E34), with the Double jet + tau seed
- created a new column 0.4E34 in the PS table for rate studies, with menu v0 +  SingleIsoTau35 activated
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v1_0_0/PrescaleTable/L1Menu_Collisions2022_v1_0_0.xlsx
+++ b/development/L1Menu_Collisions2022_v1_0_0/PrescaleTable/L1Menu_Collisions2022_v1_0_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2022_v1_0_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0900D7C-71FB-2546-8F9E-AAB9CE8FA3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C01FF80-991E-C94E-9109-5A86868CF468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2541,8 +2541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF3B8E07-BE26-384A-A4B5-1B0A96E53592}">
   <dimension ref="A1:IV382"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A152" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C168" sqref="C168"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3298,28 +3298,28 @@
         <v>0</v>
       </c>
       <c r="D22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3333,28 +3333,28 @@
         <v>0</v>
       </c>
       <c r="D23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3368,28 +3368,28 @@
         <v>0</v>
       </c>
       <c r="D24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>